<commit_message>
model almost complete, and modify the input data
</commit_message>
<xml_diff>
--- a/data/sheet.xlsx
+++ b/data/sheet.xlsx
@@ -37,8 +37,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="176" formatCode="0.00_ "/>
+    <numFmt numFmtId="177" formatCode="0.0000_ "/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -76,9 +77,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -361,8 +363,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="Z43" sqref="Z43"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C31" sqref="C1:C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -374,7 +376,7 @@
       <c r="B1">
         <v>0</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1" s="2">
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D1">
@@ -451,7 +453,7 @@
       <c r="B2">
         <v>0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="2">
         <v>0.1</v>
       </c>
       <c r="D2">
@@ -525,7 +527,7 @@
       <c r="B3">
         <v>4.1666666666666666E-3</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="2">
         <v>0.10416666666666667</v>
       </c>
       <c r="D3">
@@ -599,7 +601,7 @@
       <c r="B4">
         <v>8.3333333333333332E-3</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="2">
         <v>0.12083333333333333</v>
       </c>
       <c r="D4">
@@ -673,7 +675,7 @@
       <c r="B5">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="2">
         <v>0.14166666666666666</v>
       </c>
       <c r="D5">
@@ -747,7 +749,7 @@
       <c r="B6">
         <v>2.9166666666666667E-2</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="2">
         <v>0.14791666666666667</v>
       </c>
       <c r="D6">
@@ -821,7 +823,7 @@
       <c r="B7">
         <v>3.125E-2</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7" s="2">
         <v>0.15</v>
       </c>
       <c r="D7">
@@ -895,7 +897,7 @@
       <c r="B8">
         <v>4.3749999999999997E-2</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8" s="2">
         <v>0.17499999999999999</v>
       </c>
       <c r="D8">
@@ -969,7 +971,7 @@
       <c r="B9">
         <v>6.0416666666666667E-2</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9" s="2">
         <v>0.18333333333333332</v>
       </c>
       <c r="D9">
@@ -1043,7 +1045,7 @@
       <c r="B10">
         <v>6.8750000000000006E-2</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10" s="2">
         <v>0.23333333333333334</v>
       </c>
       <c r="D10">
@@ -1117,7 +1119,7 @@
       <c r="B11">
         <v>6.8750000000000006E-2</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11" s="2">
         <v>0.23333333333333334</v>
       </c>
       <c r="D11">
@@ -1191,7 +1193,7 @@
       <c r="B12">
         <v>7.9166666666666663E-2</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12" s="2">
         <v>0.23541666666666666</v>
       </c>
       <c r="D12">
@@ -1265,7 +1267,7 @@
       <c r="B13">
         <v>7.9166666666666663E-2</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13" s="2">
         <v>0.24583333333333332</v>
       </c>
       <c r="D13">
@@ -1339,7 +1341,7 @@
       <c r="B14">
         <v>7.9166666666666663E-2</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14" s="2">
         <v>0.25</v>
       </c>
       <c r="D14">
@@ -1413,7 +1415,7 @@
       <c r="B15">
         <v>8.7499999999999994E-2</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15" s="2">
         <v>0.30416666666666664</v>
       </c>
       <c r="D15">
@@ -1487,7 +1489,7 @@
       <c r="B16">
         <v>0.1</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16" s="2">
         <v>0.31041666666666667</v>
       </c>
       <c r="D16">
@@ -1561,7 +1563,7 @@
       <c r="B17">
         <v>0.10416666666666667</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17" s="2">
         <v>0.31458333333333333</v>
       </c>
       <c r="D17">
@@ -1635,7 +1637,7 @@
       <c r="B18">
         <v>0.12083333333333333</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18" s="2">
         <v>0.33958333333333335</v>
       </c>
       <c r="D18">
@@ -1709,7 +1711,7 @@
       <c r="B19">
         <v>0.14166666666666666</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19" s="2">
         <v>0.35208333333333336</v>
       </c>
       <c r="D19">
@@ -1783,7 +1785,7 @@
       <c r="B20">
         <v>0.14791666666666667</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20" s="2">
         <v>0.36666666666666664</v>
       </c>
       <c r="D20">
@@ -1857,7 +1859,7 @@
       <c r="B21">
         <v>0.15</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21" s="2">
         <v>0.41041666666666665</v>
       </c>
       <c r="D21">
@@ -1931,7 +1933,7 @@
       <c r="B22">
         <v>0.17499999999999999</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22" s="2">
         <v>0.43125000000000002</v>
       </c>
       <c r="D22">
@@ -2005,7 +2007,7 @@
       <c r="B23">
         <v>0.18333333333333332</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23" s="2">
         <v>0.47708333333333336</v>
       </c>
       <c r="D23">
@@ -2079,7 +2081,7 @@
       <c r="B24">
         <v>0.23333333333333334</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24" s="2">
         <v>0.47291666666666665</v>
       </c>
       <c r="D24">
@@ -2153,7 +2155,7 @@
       <c r="B25">
         <v>0.23333333333333334</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25" s="2">
         <v>0.48541666666666666</v>
       </c>
       <c r="D25">
@@ -2227,7 +2229,7 @@
       <c r="B26">
         <v>0.23541666666666666</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26" s="2">
         <v>0.48125000000000001</v>
       </c>
       <c r="D26">
@@ -2301,7 +2303,7 @@
       <c r="B27">
         <v>0.24583333333333332</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27" s="2">
         <v>0.48541666666666666</v>
       </c>
       <c r="D27">
@@ -2375,7 +2377,7 @@
       <c r="B28">
         <v>0.25</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28" s="2">
         <v>0.48125000000000001</v>
       </c>
       <c r="D28">
@@ -2449,7 +2451,7 @@
       <c r="B29">
         <v>0.30416666666666664</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29" s="2">
         <v>0.47708333333333336</v>
       </c>
       <c r="D29">
@@ -2523,7 +2525,7 @@
       <c r="B30">
         <v>0.31041666666666667</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30" s="2">
         <v>0.48749999999999999</v>
       </c>
       <c r="D30">
@@ -2597,7 +2599,7 @@
       <c r="B31">
         <v>0.31458333333333333</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31" s="2">
         <v>0.48749999999999999</v>
       </c>
       <c r="D31">
@@ -2751,8 +2753,8 @@
       <c r="B33">
         <v>0.33958333333333335</v>
       </c>
-      <c r="C33" s="1">
-        <v>3.7500000000000001E-4</v>
+      <c r="C33" s="2">
+        <v>0.46666666666666667</v>
       </c>
       <c r="D33">
         <v>0.44374999999999998</v>
@@ -2825,8 +2827,8 @@
       <c r="B34">
         <v>0.35208333333333336</v>
       </c>
-      <c r="C34" s="1">
-        <v>3.8888888888888892E-4</v>
+      <c r="C34" s="2">
+        <v>0.46666666666666667</v>
       </c>
       <c r="D34">
         <v>0.42291666666666666</v>
@@ -2899,8 +2901,8 @@
       <c r="B35">
         <v>0.36666666666666664</v>
       </c>
-      <c r="C35" s="1">
-        <v>4.3750000000000001E-4</v>
+      <c r="C35" s="2">
+        <v>0.44791666666666669</v>
       </c>
       <c r="D35">
         <v>0.44374999999999998</v>
@@ -2973,8 +2975,8 @@
       <c r="B36">
         <v>0.41041666666666665</v>
       </c>
-      <c r="C36" s="1">
-        <v>4.5833333333333332E-4</v>
+      <c r="C36" s="2">
+        <v>0.46875</v>
       </c>
       <c r="D36">
         <v>0.44791666666666669</v>
@@ -3047,8 +3049,8 @@
       <c r="B37">
         <v>0.43125000000000002</v>
       </c>
-      <c r="C37" s="1">
-        <v>4.6527777777777778E-4</v>
+      <c r="C37" s="2">
+        <v>0.47083333333333333</v>
       </c>
       <c r="D37">
         <v>0.45</v>
@@ -3121,8 +3123,8 @@
       <c r="B38">
         <v>0.47708333333333336</v>
       </c>
-      <c r="C38" s="1">
-        <v>4.5833333333333332E-4</v>
+      <c r="C38" s="2">
+        <v>0.45208333333333334</v>
       </c>
       <c r="D38">
         <v>0.42291666666666666</v>
@@ -3195,8 +3197,8 @@
       <c r="B39">
         <v>0.47291666666666665</v>
       </c>
-      <c r="C39" s="1">
-        <v>5.1736111111111112E-4</v>
+      <c r="C39" s="2">
+        <v>0.45624999999999999</v>
       </c>
       <c r="D39">
         <v>0.46041666666666664</v>
@@ -3269,8 +3271,8 @@
       <c r="B40">
         <v>0.48541666666666666</v>
       </c>
-      <c r="C40" s="1">
-        <v>5.1388888888888892E-4</v>
+      <c r="C40" s="2">
+        <v>0.46250000000000002</v>
       </c>
       <c r="D40">
         <v>0.48749999999999999</v>
@@ -3343,8 +3345,8 @@
       <c r="B41">
         <v>0.48125000000000001</v>
       </c>
-      <c r="C41" s="1">
-        <v>5.0694444444444452E-4</v>
+      <c r="C41" s="2">
+        <v>0.45208333333333334</v>
       </c>
       <c r="D41">
         <v>0.50416666666666665</v>
@@ -3417,8 +3419,8 @@
       <c r="B42">
         <v>0.48541666666666666</v>
       </c>
-      <c r="C42" s="1">
-        <v>5.4166666666666664E-4</v>
+      <c r="C42" s="2">
+        <v>0.46458333333333335</v>
       </c>
       <c r="D42">
         <v>0.49166666666666664</v>
@@ -3491,8 +3493,8 @@
       <c r="B43">
         <v>0.48125000000000001</v>
       </c>
-      <c r="C43" s="1">
-        <v>5.9027777777777778E-4</v>
+      <c r="C43" s="2">
+        <v>0.46875</v>
       </c>
       <c r="D43">
         <v>0.48749999999999999</v>
@@ -3565,8 +3567,8 @@
       <c r="B44">
         <v>0.47708333333333336</v>
       </c>
-      <c r="C44" s="1">
-        <v>6.0069444444444439E-4</v>
+      <c r="C44" s="2">
+        <v>0.44374999999999998</v>
       </c>
       <c r="D44">
         <v>0.47708333333333336</v>
@@ -3639,8 +3641,8 @@
       <c r="B45">
         <v>0.48749999999999999</v>
       </c>
-      <c r="C45" s="1">
-        <v>5.7291666666666667E-4</v>
+      <c r="C45" s="2">
+        <v>0.41458333333333336</v>
       </c>
       <c r="D45">
         <v>0.48125000000000001</v>
@@ -3713,8 +3715,8 @@
       <c r="B46">
         <v>0.48749999999999999</v>
       </c>
-      <c r="C46" s="1">
-        <v>5.6944444444444436E-4</v>
+      <c r="C46" s="2">
+        <v>0.38958333333333334</v>
       </c>
       <c r="D46">
         <v>0.48125000000000001</v>
@@ -3787,8 +3789,8 @@
       <c r="B47">
         <v>0.45833333333333331</v>
       </c>
-      <c r="C47" s="1">
-        <v>5.8333333333333338E-4</v>
+      <c r="C47" s="2">
+        <v>0.42083333333333334</v>
       </c>
       <c r="D47">
         <v>0.50208333333333333</v>

</xml_diff>